<commit_message>
Data Provider and assertions added
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sandip\eclipse-workspace\DataDrivenFramework\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8E791015-58DE-4805-A691-7AB96AC2FD60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A60C5D2-0B76-41A5-BD7F-8F5D326D8F57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B2BD0B99-DC30-4261-918E-2D9C69E7E63E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="AddCustomerTest" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,6 +30,41 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+  <si>
+    <t>firstname</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>postcode</t>
+  </si>
+  <si>
+    <t>sandip</t>
+  </si>
+  <si>
+    <t>thopate</t>
+  </si>
+  <si>
+    <t>hsf894r</t>
+  </si>
+  <si>
+    <t>lasdjf</t>
+  </si>
+  <si>
+    <t>lslsjf</t>
+  </si>
+  <si>
+    <t>alerttext</t>
+  </si>
+  <si>
+    <t>Customer added successfully</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -63,8 +98,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -379,14 +417,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9536931F-217D-4E41-B69D-4CC9B29B7F1A}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="4" max="4" width="33.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1">
+        <v>567898</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
created common data provider
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sandip\eclipse-workspace\DataDrivenFramework\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A60C5D2-0B76-41A5-BD7F-8F5D326D8F57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2841F27C-84CE-4A90-900E-412F3F1CADDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B2BD0B99-DC30-4261-918E-2D9C69E7E63E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{B2BD0B99-DC30-4261-918E-2D9C69E7E63E}"/>
   </bookViews>
   <sheets>
     <sheet name="AddCustomerTest" sheetId="1" r:id="rId1"/>
+    <sheet name="OpenAccountTest" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>firstname</t>
   </si>
@@ -50,19 +51,28 @@
     <t>thopate</t>
   </si>
   <si>
-    <t>hsf894r</t>
-  </si>
-  <si>
-    <t>lasdjf</t>
-  </si>
-  <si>
-    <t>lslsjf</t>
-  </si>
-  <si>
     <t>alerttext</t>
   </si>
   <si>
     <t>Customer added successfully</t>
+  </si>
+  <si>
+    <t>customer</t>
+  </si>
+  <si>
+    <t>currency</t>
+  </si>
+  <si>
+    <t>sandip thopate</t>
+  </si>
+  <si>
+    <t>rupee</t>
+  </si>
+  <si>
+    <t>vishal</t>
+  </si>
+  <si>
+    <t>sahu</t>
   </si>
 </sst>
 </file>
@@ -419,7 +429,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9536931F-217D-4E41-B69D-4CC9B29B7F1A}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -439,7 +449,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -449,25 +459,60 @@
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
+      <c r="C2" s="1">
+        <v>411033</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1">
+        <v>411034</v>
+      </c>
+      <c r="D3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E3F6A43-B8BA-4636-B377-FDDAC093B126}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1">
-        <v>567898</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
set up run modes for test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sandip\eclipse-workspace\DataDrivenFramework\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2841F27C-84CE-4A90-900E-412F3F1CADDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3821E507-31B0-4046-AE99-7ED9D42FA097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{B2BD0B99-DC30-4261-918E-2D9C69E7E63E}"/>
   </bookViews>
   <sheets>
-    <sheet name="AddCustomerTest" sheetId="1" r:id="rId1"/>
-    <sheet name="OpenAccountTest" sheetId="2" r:id="rId2"/>
+    <sheet name="test_suite" sheetId="3" r:id="rId1"/>
+    <sheet name="AddCustomerTest" sheetId="1" r:id="rId2"/>
+    <sheet name="OpenAccountTest" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
   <si>
     <t>firstname</t>
   </si>
@@ -66,13 +67,43 @@
     <t>sandip thopate</t>
   </si>
   <si>
-    <t>rupee</t>
-  </si>
-  <si>
     <t>vishal</t>
   </si>
   <si>
     <t>sahu</t>
+  </si>
+  <si>
+    <t>vicky</t>
+  </si>
+  <si>
+    <t>yadav</t>
+  </si>
+  <si>
+    <t>gaurav</t>
+  </si>
+  <si>
+    <t>Rupee</t>
+  </si>
+  <si>
+    <t>TCID</t>
+  </si>
+  <si>
+    <t>Runmode</t>
+  </si>
+  <si>
+    <t>BankManagerLoginTest</t>
+  </si>
+  <si>
+    <t>AddCustomerTest</t>
+  </si>
+  <si>
+    <t>OpenAccountTest</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -426,11 +457,62 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9536931F-217D-4E41-B69D-4CC9B29B7F1A}">
-  <dimension ref="A1:D3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{036BB60A-D766-4E99-B2A9-D08BFB08E9EF}">
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B1" sqref="B1:B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24.33203125" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9536931F-217D-4E41-B69D-4CC9B29B7F1A}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -468,15 +550,43 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
         <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
       </c>
       <c r="C3" s="1">
         <v>411034</v>
       </c>
       <c r="D3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>412303</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <v>412301</v>
+      </c>
+      <c r="D5" t="s">
         <v>6</v>
       </c>
     </row>
@@ -485,12 +595,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E3F6A43-B8BA-4636-B377-FDDAC093B126}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -512,7 +622,7 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>